<commit_message>
Lr routes fixed, added boolena billed, made adjustments in add and viewing lr
</commit_message>
<xml_diff>
--- a/lr.xlsx
+++ b/lr.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="My Users" state="visible" r:id="rId4"/>
+    <sheet sheetId="1" name="LR" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>S.no</t>
   </si>
@@ -52,22 +52,13 @@
     <t>2011-08-19</t>
   </si>
   <si>
-    <t>123</t>
-  </si>
-  <si>
-    <t>s</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>2011-08-07</t>
-  </si>
-  <si>
-    <t>122</t>
-  </si>
-  <si>
-    <t>12223</t>
+    <t>SS</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>13</t>
   </si>
 </sst>
 </file>
@@ -448,7 +439,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L2"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="3" width="10" customWidth="1"/>
@@ -507,63 +498,19 @@
         <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E2" t="s">
         <v>14</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" t="s">
         <v>15</v>
       </c>
+      <c r="G2">
+        <v>1234567</v>
+      </c>
       <c r="H2">
-        <v>12</v>
-      </c>
-      <c r="I2">
         <v>123</v>
-      </c>
-      <c r="J2">
-        <v>123</v>
-      </c>
-      <c r="K2">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3">
-        <v>12</v>
-      </c>
-      <c r="I3">
-        <v>123</v>
-      </c>
-      <c r="J3">
-        <v>1233</v>
-      </c>
-      <c r="K3">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mulitple Party Lr routes are being made
</commit_message>
<xml_diff>
--- a/lr.xlsx
+++ b/lr.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t>S.no</t>
   </si>
@@ -49,19 +49,31 @@
     <t>Unloading Charges</t>
   </si>
   <si>
-    <t>2021-01-22</t>
-  </si>
-  <si>
-    <t>SILI</t>
-  </si>
-  <si>
-    <t>SS</t>
+    <t>2021-01-03</t>
+  </si>
+  <si>
+    <t>SILIG</t>
+  </si>
+  <si>
+    <t>SSWW</t>
   </si>
   <si>
     <t>DARJ</t>
   </si>
   <si>
-    <t>11</t>
+    <t>13</t>
+  </si>
+  <si>
+    <t>2021-01-20</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>2011-08-19</t>
+  </si>
+  <si>
+    <t>Q</t>
   </si>
 </sst>
 </file>
@@ -442,7 +454,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L4"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="3" width="10" customWidth="1"/>
@@ -513,7 +525,71 @@
         <v>1211</v>
       </c>
       <c r="H2">
-        <v>111</v>
+        <v>111222</v>
+      </c>
+      <c r="I2">
+        <v>123</v>
+      </c>
+      <c r="J2">
+        <v>12</v>
+      </c>
+      <c r="K2">
+        <v>12212</v>
+      </c>
+      <c r="L2">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3">
+        <v>121</v>
+      </c>
+      <c r="H3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4">
+        <v>112</v>
+      </c>
+      <c r="H4">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made some changes, add multiple partylr made
</commit_message>
<xml_diff>
--- a/lr.xlsx
+++ b/lr.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>S.no</t>
   </si>
@@ -47,33 +47,6 @@
   </si>
   <si>
     <t>Unloading Charges</t>
-  </si>
-  <si>
-    <t>2021-01-03</t>
-  </si>
-  <si>
-    <t>SILIG</t>
-  </si>
-  <si>
-    <t>SSWW</t>
-  </si>
-  <si>
-    <t>DARJ</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>2021-01-20</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>2011-08-19</t>
-  </si>
-  <si>
-    <t>Q</t>
   </si>
 </sst>
 </file>
@@ -454,7 +427,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L1"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="3" width="10" customWidth="1"/>
@@ -502,96 +475,6 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2">
-        <v>1211</v>
-      </c>
-      <c r="H2">
-        <v>111222</v>
-      </c>
-      <c r="I2">
-        <v>123</v>
-      </c>
-      <c r="J2">
-        <v>12</v>
-      </c>
-      <c r="K2">
-        <v>12212</v>
-      </c>
-      <c r="L2">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3">
-        <v>121</v>
-      </c>
-      <c r="H3">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4">
-        <v>112</v>
-      </c>
-      <c r="H4">
-        <v>12</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>